<commit_message>
set up 6 and 17
</commit_message>
<xml_diff>
--- a/js/16/16.xlsx
+++ b/js/16/16.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scrich/Dev/AdventOfCode/js/16/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7DA6A8-3596-6B4E-B7AE-F65DC7808A4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A890708-ED7E-8649-9E4C-CC9C050FFEE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="1360" windowWidth="21380" windowHeight="17140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10440" yWindow="1620" windowWidth="21380" windowHeight="17140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="valid_tickets" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>zone</t>
   </si>
@@ -88,12 +89,72 @@
   <si>
     <t>min</t>
   </si>
+  <si>
+    <t>0   departure time</t>
+  </si>
+  <si>
+    <t>1   arrival station</t>
+  </si>
+  <si>
+    <t>2   departure station</t>
+  </si>
+  <si>
+    <t>3   route</t>
+  </si>
+  <si>
+    <t>4   departure track</t>
+  </si>
+  <si>
+    <t>5   arrival track</t>
+  </si>
+  <si>
+    <t>6   arrival location</t>
+  </si>
+  <si>
+    <t>7   departure location</t>
+  </si>
+  <si>
+    <t>8   price</t>
+  </si>
+  <si>
+    <t>9   departure platform</t>
+  </si>
+  <si>
+    <t>10  row</t>
+  </si>
+  <si>
+    <t>11  train</t>
+  </si>
+  <si>
+    <t>12  zone</t>
+  </si>
+  <si>
+    <t>13  type</t>
+  </si>
+  <si>
+    <t>14  duration</t>
+  </si>
+  <si>
+    <t>15  arrival platform</t>
+  </si>
+  <si>
+    <t>16  class</t>
+  </si>
+  <si>
+    <t>17  seat</t>
+  </si>
+  <si>
+    <t>18  departure date</t>
+  </si>
+  <si>
+    <t>19  wagon</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +288,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFCE9178"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="35">
@@ -582,10 +649,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1200,7 +1268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E152" workbookViewId="0">
+    <sheetView topLeftCell="E152" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:U191"/>
     </sheetView>
   </sheetViews>
@@ -13794,4 +13862,275 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BDE5B22-B51E-794F-A7F7-6CFEE0A55837}">
+  <dimension ref="A1:V30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3">
+        <v>139</v>
+      </c>
+      <c r="C1">
+        <f>B1</f>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>61</v>
+      </c>
+      <c r="C3">
+        <f>B3</f>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5">
+        <v>101</v>
+      </c>
+      <c r="C5">
+        <f>B5</f>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8">
+        <v>53</v>
+      </c>
+      <c r="C8">
+        <f>B8</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10">
+        <v>59</v>
+      </c>
+      <c r="C10">
+        <f>B10</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19">
+        <v>137</v>
+      </c>
+      <c r="C19">
+        <f>B19</f>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <f>C1*C3*C5*C8*C10*C19</f>
+        <v>366871907221</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="C30" s="3">
+        <v>139</v>
+      </c>
+      <c r="D30">
+        <v>109</v>
+      </c>
+      <c r="E30">
+        <v>61</v>
+      </c>
+      <c r="F30">
+        <v>149</v>
+      </c>
+      <c r="G30">
+        <v>101</v>
+      </c>
+      <c r="H30">
+        <v>89</v>
+      </c>
+      <c r="I30">
+        <v>103</v>
+      </c>
+      <c r="J30">
+        <v>53</v>
+      </c>
+      <c r="K30">
+        <v>107</v>
+      </c>
+      <c r="L30">
+        <v>59</v>
+      </c>
+      <c r="M30">
+        <v>73</v>
+      </c>
+      <c r="N30">
+        <v>151</v>
+      </c>
+      <c r="O30">
+        <v>71</v>
+      </c>
+      <c r="P30">
+        <v>67</v>
+      </c>
+      <c r="Q30">
+        <v>97</v>
+      </c>
+      <c r="R30">
+        <v>113</v>
+      </c>
+      <c r="S30">
+        <v>83</v>
+      </c>
+      <c r="T30">
+        <v>163</v>
+      </c>
+      <c r="U30">
+        <v>137</v>
+      </c>
+      <c r="V30">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>